<commit_message>
Diff of exp kernel + Bug Fix
Here , i have added diff of exp kernal.

Also, fixed bug where the Current Q Index was not getting properly
initialized (missing mxGetData).

Added code to automatically calculate the length of Matlab Structs in
order to avoid the hellish error.
Slightly updated procedure of adding variables

Also added the matlab code ConvertStatetoInitialCond.m .
</commit_message>
<xml_diff>
--- a/TimeDelNetSimMEX_Lib/Items/enumedit.xlsx
+++ b/TimeDelNetSimMEX_Lib/Items/enumedit.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>V_REQ</t>
   </si>
   <si>
-    <t>I_IN_REQ</t>
-  </si>
-  <si>
     <t>TIME_REQ</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>Final String</t>
+  </si>
+  <si>
+    <t>I_IN_1_REQ</t>
+  </si>
+  <si>
+    <t>I_IN_2_REQ</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,22 +417,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -452,153 +455,153 @@
         <v xml:space="preserve">V_REQ               = (1 &lt;&lt; 0), </v>
       </c>
       <c r="G2">
-        <f>MAX(C2:C13)</f>
+        <f>MAX(C2:C14)</f>
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C13" si="0">LEN(A3)</f>
-        <v>8</v>
+        <f t="shared" ref="C3:C14" si="0">LEN(A3)</f>
+        <v>10</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D13" si="1">CONCATENATE(A3, REPT(" ",$G$2+1-C3))</f>
-        <v xml:space="preserve">I_IN_REQ           </v>
+        <f t="shared" ref="D3:D14" si="1">CONCATENATE(A3, REPT(" ",$G$2+1-C3))</f>
+        <v xml:space="preserve">I_IN_1_REQ         </v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E13" si="2">CONCATENATE(D3," = (1 &lt;&lt; ",B3,"), ")</f>
-        <v xml:space="preserve">I_IN_REQ            = (1 &lt;&lt; 1), </v>
+        <f t="shared" ref="E3:E14" si="2">CONCATENATE(D3," = (1 &lt;&lt; ",B3,"), ")</f>
+        <v xml:space="preserve">I_IN_1_REQ          = (1 &lt;&lt; 1), </v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" ref="C4" si="3">LEN(A4)</f>
+        <v>10</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">TIME_REQ           </v>
+        <f t="shared" ref="D4" si="4">CONCATENATE(A4, REPT(" ",$G$2+1-C4))</f>
+        <v xml:space="preserve">I_IN_2_REQ         </v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">TIME_REQ            = (1 &lt;&lt; 2), </v>
+        <f t="shared" ref="E4" si="5">CONCATENATE(D4," = (1 &lt;&lt; ",B4,"), ")</f>
+        <v xml:space="preserve">I_IN_2_REQ          = (1 &lt;&lt; 2), </v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">U_REQ              </v>
+        <v xml:space="preserve">TIME_REQ           </v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">U_REQ               = (1 &lt;&lt; 3), </v>
+        <v xml:space="preserve">TIME_REQ            = (1 &lt;&lt; 3), </v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">WEIGHT_REQ         </v>
+        <v xml:space="preserve">U_REQ              </v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">WEIGHT_REQ          = (1 &lt;&lt; 4), </v>
+        <v xml:space="preserve">U_REQ               = (1 &lt;&lt; 4), </v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">CURRENT_QINDS_REQ  </v>
+        <v xml:space="preserve">WEIGHT_REQ         </v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">CURRENT_QINDS_REQ   = (1 &lt;&lt; 5), </v>
+        <v xml:space="preserve">WEIGHT_REQ          = (1 &lt;&lt; 5), </v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">SPIKE_QUEUE_REQ    </v>
+        <v xml:space="preserve">CURRENT_QINDS_REQ  </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">SPIKE_QUEUE_REQ     = (1 &lt;&lt; 6), </v>
+        <v xml:space="preserve">CURRENT_QINDS_REQ   = (1 &lt;&lt; 6), </v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">LASTSPIKED_NEU_REQ </v>
+        <v xml:space="preserve">SPIKE_QUEUE_REQ    </v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">LASTSPIKED_NEU_REQ  = (1 &lt;&lt; 7), </v>
+        <v xml:space="preserve">SPIKE_QUEUE_REQ     = (1 &lt;&lt; 7), </v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -609,71 +612,91 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">LASTSPIKED_SYN_REQ </v>
+        <v xml:space="preserve">LASTSPIKED_NEU_REQ </v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">LASTSPIKED_SYN_REQ  = (1 &lt;&lt; 8), </v>
+        <v xml:space="preserve">LASTSPIKED_NEU_REQ  = (1 &lt;&lt; 8), </v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">I_TOT_REQ          </v>
+        <v xml:space="preserve">LASTSPIKED_SYN_REQ </v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">I_TOT_REQ           = (1 &lt;&lt; 9), </v>
+        <v xml:space="preserve">LASTSPIKED_SYN_REQ  = (1 &lt;&lt; 9), </v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">INITIAL_STATE_REQ  </v>
+        <v xml:space="preserve">I_TOT_REQ          </v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">INITIAL_STATE_REQ   = (1 &lt;&lt; 10), </v>
+        <v xml:space="preserve">I_TOT_REQ           = (1 &lt;&lt; 10), </v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">INITIAL_STATE_REQ  </v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">INITIAL_STATE_REQ   = (1 &lt;&lt; 11), </v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">FINAL_STATE_REQ    </v>
       </c>
-      <c r="E13" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">FINAL_STATE_REQ     = (1 &lt;&lt; 11), </v>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">FINAL_STATE_REQ     = (1 &lt;&lt; 12), </v>
       </c>
     </row>
   </sheetData>

</xml_diff>